<commit_message>
Reading Survey 170308 added
</commit_message>
<xml_diff>
--- a/data/reading_1701.xlsx
+++ b/data/reading_1701.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\★생활속의통계학★\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/coop2711/Google 드라이브/Works/Class/Statistics/R.WD/Class_data/class201701/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11775" yWindow="4365" windowWidth="28800" windowHeight="17595" tabRatio="500"/>
+    <workbookView xWindow="-34420" yWindow="2980" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="시트1" sheetId="1" r:id="rId1"/>
@@ -1872,7 +1872,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1961,16 +1961,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2057,13 +2057,13 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -2083,7 +2083,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2107,19 +2107,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2133,25 +2143,33 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="기본" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -2431,39 +2449,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU166"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="A148" sqref="A148:XFD148"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" customWidth="1"/>
-    <col min="2" max="2" width="8.5546875" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
-    <col min="7" max="7" width="28.5546875" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="28.5703125" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="23"/>
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="14"/>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
+      <c r="B2" s="27"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -2480,48 +2498,48 @@
       <c r="L2" s="7" t="s">
         <v>521</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="M2" s="15" t="s">
         <v>523</v>
       </c>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="15" t="s">
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="18" t="s">
         <v>524</v>
       </c>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25"/>
-      <c r="T2" s="16"/>
-      <c r="U2" s="17" t="s">
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="21" t="s">
         <v>525</v>
       </c>
-      <c r="V2" s="17"/>
-      <c r="W2" s="17" t="s">
+      <c r="V2" s="21"/>
+      <c r="W2" s="21" t="s">
         <v>526</v>
       </c>
-      <c r="X2" s="17"/>
+      <c r="X2" s="21"/>
       <c r="Y2" s="7" t="s">
         <v>527</v>
       </c>
-      <c r="Z2" s="17" t="s">
+      <c r="Z2" s="21" t="s">
         <v>528</v>
       </c>
-      <c r="AA2" s="17"/>
-      <c r="AB2" s="17" t="s">
+      <c r="AA2" s="21"/>
+      <c r="AB2" s="21" t="s">
         <v>529</v>
       </c>
-      <c r="AC2" s="17"/>
+      <c r="AC2" s="21"/>
       <c r="AD2" s="7" t="s">
         <v>530</v>
       </c>
-      <c r="AE2" s="17" t="s">
+      <c r="AE2" s="21" t="s">
         <v>531</v>
       </c>
-      <c r="AF2" s="17"/>
-      <c r="AG2" s="17"/>
-      <c r="AH2" s="17"/>
-      <c r="AI2" s="17"/>
-      <c r="AJ2" s="17"/>
+      <c r="AF2" s="21"/>
+      <c r="AG2" s="21"/>
+      <c r="AH2" s="21"/>
+      <c r="AI2" s="21"/>
+      <c r="AJ2" s="21"/>
       <c r="AK2" s="7" t="s">
         <v>532</v>
       </c>
@@ -2530,12 +2548,12 @@
         <v>533</v>
       </c>
       <c r="AN2" s="7"/>
-      <c r="AO2" s="20" t="s">
+      <c r="AO2" s="24" t="s">
         <v>534</v>
       </c>
-      <c r="AP2" s="20"/>
-      <c r="AQ2" s="20"/>
-      <c r="AR2" s="20"/>
+      <c r="AP2" s="24"/>
+      <c r="AQ2" s="24"/>
+      <c r="AR2" s="24"/>
       <c r="AS2" s="7" t="s">
         <v>535</v>
       </c>
@@ -2544,7 +2562,7 @@
       </c>
       <c r="AU2" s="6"/>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -2557,22 +2575,22 @@
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
-      <c r="M3" s="11" t="s">
+      <c r="M3" s="25" t="s">
         <v>537</v>
       </c>
-      <c r="N3" s="12"/>
-      <c r="O3" s="13" t="s">
+      <c r="N3" s="26"/>
+      <c r="O3" s="15" t="s">
         <v>538</v>
       </c>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="15" t="s">
+      <c r="P3" s="17"/>
+      <c r="Q3" s="18" t="s">
         <v>537</v>
       </c>
-      <c r="R3" s="16"/>
-      <c r="S3" s="18" t="s">
+      <c r="R3" s="20"/>
+      <c r="S3" s="22" t="s">
         <v>538</v>
       </c>
-      <c r="T3" s="19"/>
+      <c r="T3" s="23"/>
       <c r="U3" s="7" t="s">
         <v>540</v>
       </c>
@@ -2599,16 +2617,16 @@
         <v>543</v>
       </c>
       <c r="AD3" s="7"/>
-      <c r="AE3" s="17" t="s">
+      <c r="AE3" s="21" t="s">
         <v>542</v>
       </c>
-      <c r="AF3" s="17"/>
-      <c r="AG3" s="17"/>
-      <c r="AH3" s="17" t="s">
+      <c r="AF3" s="21"/>
+      <c r="AG3" s="21"/>
+      <c r="AH3" s="21" t="s">
         <v>543</v>
       </c>
-      <c r="AI3" s="17"/>
-      <c r="AJ3" s="17"/>
+      <c r="AI3" s="21"/>
+      <c r="AJ3" s="21"/>
       <c r="AK3" s="7" t="s">
         <v>539</v>
       </c>
@@ -2621,19 +2639,19 @@
       <c r="AN3" s="7" t="s">
         <v>541</v>
       </c>
-      <c r="AO3" s="17" t="s">
+      <c r="AO3" s="21" t="s">
         <v>544</v>
       </c>
-      <c r="AP3" s="17"/>
-      <c r="AQ3" s="17" t="s">
+      <c r="AP3" s="21"/>
+      <c r="AQ3" s="21" t="s">
         <v>545</v>
       </c>
-      <c r="AR3" s="17"/>
+      <c r="AR3" s="21"/>
       <c r="AS3" s="7"/>
       <c r="AT3" s="7"/>
       <c r="AU3" s="6"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -2776,7 +2794,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -2909,7 +2927,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -3048,7 +3066,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -3187,7 +3205,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>4</v>
       </c>
@@ -3326,7 +3344,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>5</v>
       </c>
@@ -3455,7 +3473,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>6</v>
       </c>
@@ -3582,7 +3600,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>7</v>
       </c>
@@ -3721,7 +3739,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>8</v>
       </c>
@@ -3860,7 +3878,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>9</v>
       </c>
@@ -3999,7 +4017,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>10</v>
       </c>
@@ -4064,7 +4082,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>11</v>
       </c>
@@ -4193,7 +4211,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>12</v>
       </c>
@@ -4320,7 +4338,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>13</v>
       </c>
@@ -4459,7 +4477,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>14</v>
       </c>
@@ -4598,7 +4616,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>15</v>
       </c>
@@ -4733,7 +4751,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>16</v>
       </c>
@@ -4862,7 +4880,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>17</v>
       </c>
@@ -4999,7 +5017,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>18</v>
       </c>
@@ -5138,7 +5156,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>19</v>
       </c>
@@ -5277,146 +5295,146 @@
         <v>582</v>
       </c>
     </row>
-    <row r="24" spans="1:47" ht="27.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
+    <row r="24" spans="1:47" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="28">
         <v>20</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="2" t="s">
+      <c r="B24" s="29"/>
+      <c r="C24" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="28">
         <v>20175304</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="F24" s="2">
-        <v>1</v>
-      </c>
-      <c r="G24" s="2" t="s">
+      <c r="F24" s="28">
+        <v>1</v>
+      </c>
+      <c r="G24" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="H24" s="1"/>
-      <c r="I24" s="3" t="s">
+      <c r="H24" s="29"/>
+      <c r="I24" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="J24" s="6">
+      <c r="J24" s="31">
         <v>18</v>
       </c>
-      <c r="K24" s="6">
-        <v>1</v>
-      </c>
-      <c r="L24" s="6">
+      <c r="K24" s="31">
+        <v>1</v>
+      </c>
+      <c r="L24" s="31">
         <v>9</v>
       </c>
-      <c r="M24" s="6">
-        <v>3</v>
-      </c>
-      <c r="N24" s="6">
+      <c r="M24" s="31">
+        <v>3</v>
+      </c>
+      <c r="N24" s="31">
         <v>40</v>
       </c>
-      <c r="O24" s="6">
+      <c r="O24" s="31">
         <v>10</v>
       </c>
-      <c r="P24" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="6">
-        <v>0</v>
-      </c>
-      <c r="R24" s="6">
+      <c r="P24" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="31">
+        <v>0</v>
+      </c>
+      <c r="R24" s="31">
         <v>30</v>
       </c>
-      <c r="S24" s="6">
-        <v>1</v>
-      </c>
-      <c r="T24" s="6">
+      <c r="S24" s="31">
+        <v>1</v>
+      </c>
+      <c r="T24" s="31">
         <v>30</v>
       </c>
-      <c r="U24" s="6">
-        <v>1</v>
-      </c>
-      <c r="V24" s="6">
-        <v>4</v>
-      </c>
-      <c r="W24" s="6">
-        <v>3</v>
-      </c>
-      <c r="X24" s="6">
-        <v>4</v>
-      </c>
-      <c r="Y24" s="6">
-        <v>1</v>
-      </c>
-      <c r="Z24" s="6">
-        <v>2</v>
-      </c>
-      <c r="AA24" s="6">
+      <c r="U24" s="31">
+        <v>1</v>
+      </c>
+      <c r="V24" s="31">
+        <v>4</v>
+      </c>
+      <c r="W24" s="31">
+        <v>3</v>
+      </c>
+      <c r="X24" s="31">
+        <v>4</v>
+      </c>
+      <c r="Y24" s="31">
+        <v>1</v>
+      </c>
+      <c r="Z24" s="31">
+        <v>2</v>
+      </c>
+      <c r="AA24" s="31">
         <v>6</v>
       </c>
-      <c r="AB24" s="6">
+      <c r="AB24" s="31">
         <v>9</v>
       </c>
-      <c r="AC24" s="6">
+      <c r="AC24" s="31">
         <v>6</v>
       </c>
-      <c r="AD24" s="6">
-        <v>5</v>
-      </c>
-      <c r="AE24" s="6">
-        <v>3</v>
-      </c>
-      <c r="AF24" s="6">
-        <v>5</v>
-      </c>
-      <c r="AG24" s="6">
+      <c r="AD24" s="31">
+        <v>5</v>
+      </c>
+      <c r="AE24" s="31">
+        <v>3</v>
+      </c>
+      <c r="AF24" s="31">
+        <v>5</v>
+      </c>
+      <c r="AG24" s="31">
         <v>11</v>
       </c>
-      <c r="AH24" s="6">
-        <v>2</v>
-      </c>
-      <c r="AI24" s="6">
+      <c r="AH24" s="31">
+        <v>2</v>
+      </c>
+      <c r="AI24" s="31">
         <v>6</v>
       </c>
-      <c r="AJ24" s="6">
+      <c r="AJ24" s="31">
         <v>7</v>
       </c>
-      <c r="AK24" s="6">
-        <v>4</v>
-      </c>
-      <c r="AL24" s="6">
-        <v>5</v>
-      </c>
-      <c r="AM24" s="6">
+      <c r="AK24" s="31">
+        <v>4</v>
+      </c>
+      <c r="AL24" s="31">
+        <v>5</v>
+      </c>
+      <c r="AM24" s="31">
         <v>7</v>
       </c>
-      <c r="AN24" s="6">
-        <v>2</v>
-      </c>
-      <c r="AO24" s="6">
-        <v>3</v>
-      </c>
-      <c r="AP24" s="6">
-        <v>1</v>
-      </c>
-      <c r="AQ24" s="6">
-        <v>2</v>
-      </c>
-      <c r="AR24" s="6">
-        <v>1</v>
-      </c>
-      <c r="AS24" s="6">
-        <v>4</v>
-      </c>
-      <c r="AT24" s="6">
-        <v>2</v>
-      </c>
-      <c r="AU24" s="6" t="s">
+      <c r="AN24" s="31">
+        <v>2</v>
+      </c>
+      <c r="AO24" s="31">
+        <v>3</v>
+      </c>
+      <c r="AP24" s="31">
+        <v>1</v>
+      </c>
+      <c r="AQ24" s="31">
+        <v>2</v>
+      </c>
+      <c r="AR24" s="31">
+        <v>1</v>
+      </c>
+      <c r="AS24" s="31">
+        <v>4</v>
+      </c>
+      <c r="AT24" s="31">
+        <v>2</v>
+      </c>
+      <c r="AU24" s="31" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>21</v>
       </c>
@@ -5481,7 +5499,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>22</v>
       </c>
@@ -5610,7 +5628,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>23</v>
       </c>
@@ -5739,7 +5757,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>24</v>
       </c>
@@ -5878,7 +5896,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>25</v>
       </c>
@@ -6017,7 +6035,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>26</v>
       </c>
@@ -6082,7 +6100,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>27</v>
       </c>
@@ -6215,7 +6233,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>28</v>
       </c>
@@ -6354,7 +6372,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>29</v>
       </c>
@@ -6493,7 +6511,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>30</v>
       </c>
@@ -6622,7 +6640,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>31</v>
       </c>
@@ -6761,7 +6779,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>32</v>
       </c>
@@ -6900,7 +6918,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="37" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>33</v>
       </c>
@@ -7033,7 +7051,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="38" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>34</v>
       </c>
@@ -7172,7 +7190,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="39" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>35</v>
       </c>
@@ -7309,7 +7327,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="40" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>36</v>
       </c>
@@ -7448,7 +7466,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="41" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>37</v>
       </c>
@@ -7577,7 +7595,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="42" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>38</v>
       </c>
@@ -7706,7 +7724,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="43" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>39</v>
       </c>
@@ -7835,7 +7853,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="44" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>40</v>
       </c>
@@ -7974,7 +7992,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="45" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>41</v>
       </c>
@@ -8113,7 +8131,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="46" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>42</v>
       </c>
@@ -8242,7 +8260,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="47" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>43</v>
       </c>
@@ -8381,7 +8399,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="48" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>44</v>
       </c>
@@ -8520,7 +8538,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="49" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>45</v>
       </c>
@@ -8659,7 +8677,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="50" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>46</v>
       </c>
@@ -8768,7 +8786,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="51" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>47</v>
       </c>
@@ -8907,7 +8925,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="52" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>48</v>
       </c>
@@ -9034,7 +9052,7 @@
       </c>
       <c r="AU52" s="6"/>
     </row>
-    <row r="53" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>49</v>
       </c>
@@ -9163,7 +9181,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="54" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>50</v>
       </c>
@@ -9302,7 +9320,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="55" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>51</v>
       </c>
@@ -9437,7 +9455,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="56" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>52</v>
       </c>
@@ -9576,7 +9594,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="57" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>53</v>
       </c>
@@ -9709,7 +9727,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="58" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>54</v>
       </c>
@@ -9848,140 +9866,140 @@
         <v>581</v>
       </c>
     </row>
-    <row r="59" spans="1:47" ht="27.75" x14ac:dyDescent="0.3">
-      <c r="A59" s="2">
+    <row r="59" spans="1:47" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="28">
         <v>55</v>
       </c>
-      <c r="B59" s="1"/>
-      <c r="C59" s="2" t="s">
+      <c r="B59" s="29"/>
+      <c r="C59" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="D59" s="2">
+      <c r="D59" s="28">
         <v>20175312</v>
       </c>
-      <c r="E59" s="2" t="s">
+      <c r="E59" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="F59" s="2">
-        <v>1</v>
-      </c>
-      <c r="G59" s="2" t="s">
+      <c r="F59" s="28">
+        <v>1</v>
+      </c>
+      <c r="G59" s="28" t="s">
         <v>190</v>
       </c>
-      <c r="H59" s="1"/>
-      <c r="I59" s="3" t="s">
+      <c r="H59" s="29"/>
+      <c r="I59" s="30" t="s">
         <v>191</v>
       </c>
-      <c r="J59" s="6">
+      <c r="J59" s="31">
         <v>18</v>
       </c>
-      <c r="K59" s="6">
-        <v>1</v>
-      </c>
-      <c r="L59" s="6">
+      <c r="K59" s="31">
+        <v>1</v>
+      </c>
+      <c r="L59" s="31">
         <v>9</v>
       </c>
-      <c r="M59" s="6">
-        <v>3</v>
-      </c>
-      <c r="N59" s="6">
-        <v>0</v>
-      </c>
-      <c r="O59" s="6">
+      <c r="M59" s="31">
+        <v>3</v>
+      </c>
+      <c r="N59" s="31">
+        <v>0</v>
+      </c>
+      <c r="O59" s="31">
         <v>8</v>
       </c>
-      <c r="P59" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q59" s="6">
-        <v>1</v>
-      </c>
-      <c r="R59" s="6">
+      <c r="P59" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q59" s="31">
+        <v>1</v>
+      </c>
+      <c r="R59" s="31">
         <v>40</v>
       </c>
-      <c r="S59" s="6">
-        <v>3</v>
-      </c>
-      <c r="T59" s="6">
-        <v>0</v>
-      </c>
-      <c r="U59" s="6">
-        <v>1</v>
-      </c>
-      <c r="V59" s="6">
-        <v>3</v>
-      </c>
-      <c r="W59" s="6">
-        <v>5</v>
-      </c>
-      <c r="X59" s="6">
+      <c r="S59" s="31">
+        <v>3</v>
+      </c>
+      <c r="T59" s="31">
+        <v>0</v>
+      </c>
+      <c r="U59" s="31">
+        <v>1</v>
+      </c>
+      <c r="V59" s="31">
+        <v>3</v>
+      </c>
+      <c r="W59" s="31">
+        <v>5</v>
+      </c>
+      <c r="X59" s="31">
         <v>7</v>
       </c>
-      <c r="Y59" s="6">
-        <v>3</v>
-      </c>
-      <c r="Z59" s="6">
-        <v>5</v>
-      </c>
-      <c r="AA59" s="6">
+      <c r="Y59" s="31">
+        <v>3</v>
+      </c>
+      <c r="Z59" s="31">
+        <v>5</v>
+      </c>
+      <c r="AA59" s="31">
         <v>9</v>
       </c>
-      <c r="AB59" s="6">
-        <v>3</v>
-      </c>
-      <c r="AC59" s="6">
+      <c r="AB59" s="31">
+        <v>3</v>
+      </c>
+      <c r="AC59" s="31">
         <v>7</v>
       </c>
-      <c r="AD59" s="6">
-        <v>3</v>
-      </c>
-      <c r="AE59" s="6">
+      <c r="AD59" s="31">
+        <v>3</v>
+      </c>
+      <c r="AE59" s="31">
         <v>13</v>
       </c>
-      <c r="AF59" s="6">
+      <c r="AF59" s="31">
         <v>11</v>
       </c>
-      <c r="AG59" s="6">
-        <v>5</v>
-      </c>
-      <c r="AH59" s="6">
-        <v>2</v>
-      </c>
-      <c r="AI59" s="6"/>
-      <c r="AJ59" s="6"/>
-      <c r="AK59" s="6">
-        <v>1</v>
-      </c>
-      <c r="AL59" s="6">
+      <c r="AG59" s="31">
+        <v>5</v>
+      </c>
+      <c r="AH59" s="31">
+        <v>2</v>
+      </c>
+      <c r="AI59" s="31"/>
+      <c r="AJ59" s="31"/>
+      <c r="AK59" s="31">
+        <v>1</v>
+      </c>
+      <c r="AL59" s="31">
         <v>10</v>
       </c>
-      <c r="AM59" s="6">
-        <v>5</v>
-      </c>
-      <c r="AN59" s="6">
-        <v>2</v>
-      </c>
-      <c r="AO59" s="6">
-        <v>1</v>
-      </c>
-      <c r="AP59" s="6"/>
-      <c r="AQ59" s="6">
-        <v>5</v>
-      </c>
-      <c r="AR59" s="6">
-        <v>3</v>
-      </c>
-      <c r="AS59" s="6">
-        <v>4</v>
-      </c>
-      <c r="AT59" s="6">
-        <v>4</v>
-      </c>
-      <c r="AU59" s="6" t="s">
+      <c r="AM59" s="31">
+        <v>5</v>
+      </c>
+      <c r="AN59" s="31">
+        <v>2</v>
+      </c>
+      <c r="AO59" s="31">
+        <v>1</v>
+      </c>
+      <c r="AP59" s="31"/>
+      <c r="AQ59" s="31">
+        <v>5</v>
+      </c>
+      <c r="AR59" s="31">
+        <v>3</v>
+      </c>
+      <c r="AS59" s="31">
+        <v>4</v>
+      </c>
+      <c r="AT59" s="31">
+        <v>4</v>
+      </c>
+      <c r="AU59" s="31" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="60" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>56</v>
       </c>
@@ -10120,7 +10138,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="61" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>57</v>
       </c>
@@ -10259,7 +10277,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="62" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>58</v>
       </c>
@@ -10388,7 +10406,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="63" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>59</v>
       </c>
@@ -10517,7 +10535,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="64" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>60</v>
       </c>
@@ -10652,7 +10670,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="65" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>61</v>
       </c>
@@ -10717,7 +10735,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="66" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>62</v>
       </c>
@@ -10856,7 +10874,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="67" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>63</v>
       </c>
@@ -10963,7 +10981,7 @@
       </c>
       <c r="AU67" s="6"/>
     </row>
-    <row r="68" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>64</v>
       </c>
@@ -11090,7 +11108,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="69" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>65</v>
       </c>
@@ -11219,7 +11237,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="70" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>66</v>
       </c>
@@ -11358,7 +11376,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="71" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>67</v>
       </c>
@@ -11497,7 +11515,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="72" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>68</v>
       </c>
@@ -11636,7 +11654,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="73" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>69</v>
       </c>
@@ -11775,7 +11793,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="74" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>70</v>
       </c>
@@ -11840,7 +11858,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="75" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>71</v>
       </c>
@@ -11969,7 +11987,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="76" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>72</v>
       </c>
@@ -12108,7 +12126,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="77" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>73</v>
       </c>
@@ -12237,7 +12255,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="78" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>74</v>
       </c>
@@ -12372,7 +12390,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="79" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>75</v>
       </c>
@@ -12509,7 +12527,7 @@
       </c>
       <c r="AU79" s="6"/>
     </row>
-    <row r="80" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>76</v>
       </c>
@@ -12644,7 +12662,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="81" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>77</v>
       </c>
@@ -12783,7 +12801,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="82" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>78</v>
       </c>
@@ -12922,7 +12940,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="83" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>79</v>
       </c>
@@ -13055,7 +13073,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="84" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>80</v>
       </c>
@@ -13184,7 +13202,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="85" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>81</v>
       </c>
@@ -13319,7 +13337,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="86" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>82</v>
       </c>
@@ -13384,7 +13402,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="87" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>83</v>
       </c>
@@ -13513,7 +13531,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="88" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>84</v>
       </c>
@@ -13650,7 +13668,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="89" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>85</v>
       </c>
@@ -13789,7 +13807,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="90" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>86</v>
       </c>
@@ -13928,7 +13946,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="91" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>87</v>
       </c>
@@ -14057,7 +14075,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="92" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>88</v>
       </c>
@@ -14196,7 +14214,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="93" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>89</v>
       </c>
@@ -14325,7 +14343,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="94" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>90</v>
       </c>
@@ -14436,7 +14454,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="95" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>91</v>
       </c>
@@ -14501,7 +14519,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="96" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>92</v>
       </c>
@@ -14640,7 +14658,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="97" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>93</v>
       </c>
@@ -14775,7 +14793,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="98" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>94</v>
       </c>
@@ -14910,7 +14928,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="99" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>95</v>
       </c>
@@ -15049,7 +15067,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="100" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>96</v>
       </c>
@@ -15188,7 +15206,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="101" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>97</v>
       </c>
@@ -15327,7 +15345,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="102" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>98</v>
       </c>
@@ -15466,7 +15484,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="103" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>99</v>
       </c>
@@ -15575,7 +15593,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="104" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>100</v>
       </c>
@@ -15710,7 +15728,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="105" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>101</v>
       </c>
@@ -15849,7 +15867,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="106" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>102</v>
       </c>
@@ -15988,7 +16006,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="107" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>103</v>
       </c>
@@ -16125,7 +16143,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="108" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>104</v>
       </c>
@@ -16264,7 +16282,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="109" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>105</v>
       </c>
@@ -16373,7 +16391,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="110" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>106</v>
       </c>
@@ -16512,7 +16530,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="111" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>107</v>
       </c>
@@ -16641,7 +16659,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="112" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>108</v>
       </c>
@@ -16776,7 +16794,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="113" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>109</v>
       </c>
@@ -16889,7 +16907,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="114" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>110</v>
       </c>
@@ -16954,7 +16972,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="115" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>111</v>
       </c>
@@ -17019,142 +17037,142 @@
         <v>582</v>
       </c>
     </row>
-    <row r="116" spans="1:47" ht="27.75" x14ac:dyDescent="0.3">
-      <c r="A116" s="2">
+    <row r="116" spans="1:47" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="28">
         <v>112</v>
       </c>
-      <c r="B116" s="1"/>
-      <c r="C116" s="2" t="s">
+      <c r="B116" s="29"/>
+      <c r="C116" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="D116" s="2">
+      <c r="D116" s="28">
         <v>20135339</v>
       </c>
-      <c r="E116" s="2" t="s">
+      <c r="E116" s="28" t="s">
         <v>367</v>
       </c>
-      <c r="F116" s="2">
-        <v>3</v>
-      </c>
-      <c r="G116" s="2" t="s">
+      <c r="F116" s="28">
+        <v>3</v>
+      </c>
+      <c r="G116" s="28" t="s">
         <v>368</v>
       </c>
-      <c r="H116" s="1"/>
-      <c r="I116" s="3" t="s">
+      <c r="H116" s="29"/>
+      <c r="I116" s="30" t="s">
         <v>369</v>
       </c>
-      <c r="J116" s="6">
+      <c r="J116" s="31">
         <v>23</v>
       </c>
-      <c r="K116" s="6">
-        <v>1</v>
-      </c>
-      <c r="L116" s="6">
+      <c r="K116" s="31">
+        <v>1</v>
+      </c>
+      <c r="L116" s="31">
         <v>9</v>
       </c>
-      <c r="M116" s="6">
-        <v>4</v>
-      </c>
-      <c r="N116" s="6">
-        <v>0</v>
-      </c>
-      <c r="O116" s="6">
+      <c r="M116" s="31">
+        <v>4</v>
+      </c>
+      <c r="N116" s="31">
+        <v>0</v>
+      </c>
+      <c r="O116" s="31">
         <v>8</v>
       </c>
-      <c r="P116" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q116" s="6">
-        <v>0</v>
-      </c>
-      <c r="R116" s="6">
-        <v>0</v>
-      </c>
-      <c r="S116" s="6">
-        <v>0</v>
-      </c>
-      <c r="T116" s="6">
-        <v>0</v>
-      </c>
-      <c r="U116" s="6">
-        <v>1</v>
-      </c>
-      <c r="V116" s="6">
-        <v>4</v>
-      </c>
-      <c r="W116" s="6">
-        <v>4</v>
-      </c>
-      <c r="X116" s="6">
+      <c r="P116" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q116" s="31">
+        <v>0</v>
+      </c>
+      <c r="R116" s="31">
+        <v>0</v>
+      </c>
+      <c r="S116" s="31">
+        <v>0</v>
+      </c>
+      <c r="T116" s="31">
+        <v>0</v>
+      </c>
+      <c r="U116" s="31">
+        <v>1</v>
+      </c>
+      <c r="V116" s="31">
+        <v>4</v>
+      </c>
+      <c r="W116" s="31">
+        <v>4</v>
+      </c>
+      <c r="X116" s="31">
         <v>7</v>
       </c>
-      <c r="Y116" s="6">
-        <v>3</v>
-      </c>
-      <c r="Z116" s="6">
+      <c r="Y116" s="31">
+        <v>3</v>
+      </c>
+      <c r="Z116" s="31">
         <v>10</v>
       </c>
-      <c r="AA116" s="6">
+      <c r="AA116" s="31">
         <v>6</v>
       </c>
-      <c r="AB116" s="6">
-        <v>2</v>
-      </c>
-      <c r="AC116" s="6">
-        <v>0</v>
-      </c>
-      <c r="AD116" s="6">
-        <v>5</v>
-      </c>
-      <c r="AE116" s="6">
-        <v>1</v>
-      </c>
-      <c r="AF116" s="6">
-        <v>2</v>
-      </c>
-      <c r="AG116" s="6">
+      <c r="AB116" s="31">
+        <v>2</v>
+      </c>
+      <c r="AC116" s="31">
+        <v>0</v>
+      </c>
+      <c r="AD116" s="31">
+        <v>5</v>
+      </c>
+      <c r="AE116" s="31">
+        <v>1</v>
+      </c>
+      <c r="AF116" s="31">
+        <v>2</v>
+      </c>
+      <c r="AG116" s="31">
         <v>10</v>
       </c>
-      <c r="AH116" s="6">
+      <c r="AH116" s="31">
         <v>11</v>
       </c>
-      <c r="AI116" s="6">
+      <c r="AI116" s="31">
         <v>8</v>
       </c>
-      <c r="AJ116" s="6">
+      <c r="AJ116" s="31">
         <v>10</v>
       </c>
-      <c r="AK116" s="6">
-        <v>5</v>
-      </c>
-      <c r="AL116" s="6">
-        <v>2</v>
-      </c>
-      <c r="AM116" s="6">
-        <v>2</v>
-      </c>
-      <c r="AN116" s="6">
-        <v>3</v>
-      </c>
-      <c r="AO116" s="6">
+      <c r="AK116" s="31">
+        <v>5</v>
+      </c>
+      <c r="AL116" s="31">
+        <v>2</v>
+      </c>
+      <c r="AM116" s="31">
+        <v>2</v>
+      </c>
+      <c r="AN116" s="31">
+        <v>3</v>
+      </c>
+      <c r="AO116" s="31">
         <v>6</v>
       </c>
-      <c r="AP116" s="6">
-        <v>1</v>
-      </c>
-      <c r="AQ116" s="6"/>
-      <c r="AR116" s="6"/>
-      <c r="AS116" s="6">
-        <v>5</v>
-      </c>
-      <c r="AT116" s="6">
-        <v>2</v>
-      </c>
-      <c r="AU116" s="6" t="s">
+      <c r="AP116" s="31">
+        <v>1</v>
+      </c>
+      <c r="AQ116" s="31"/>
+      <c r="AR116" s="31"/>
+      <c r="AS116" s="31">
+        <v>5</v>
+      </c>
+      <c r="AT116" s="31">
+        <v>2</v>
+      </c>
+      <c r="AU116" s="31" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="117" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>113</v>
       </c>
@@ -17287,7 +17305,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="118" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>114</v>
       </c>
@@ -17422,7 +17440,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="119" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>115</v>
       </c>
@@ -17561,7 +17579,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="120" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>116</v>
       </c>
@@ -17700,7 +17718,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="121" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>117</v>
       </c>
@@ -17827,7 +17845,7 @@
       </c>
       <c r="AU121" s="6"/>
     </row>
-    <row r="122" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>118</v>
       </c>
@@ -17890,7 +17908,7 @@
       <c r="AT122" s="6"/>
       <c r="AU122" s="6"/>
     </row>
-    <row r="123" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>119</v>
       </c>
@@ -18029,7 +18047,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="124" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>120</v>
       </c>
@@ -18158,7 +18176,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="125" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>121</v>
       </c>
@@ -18297,7 +18315,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="126" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>122</v>
       </c>
@@ -18436,7 +18454,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="127" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>123</v>
       </c>
@@ -18565,146 +18583,146 @@
         <v>582</v>
       </c>
     </row>
-    <row r="128" spans="1:47" ht="27.75" x14ac:dyDescent="0.3">
-      <c r="A128" s="2">
+    <row r="128" spans="1:47" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="28">
         <v>124</v>
       </c>
-      <c r="B128" s="1"/>
-      <c r="C128" s="2" t="s">
+      <c r="B128" s="29"/>
+      <c r="C128" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="D128" s="2">
+      <c r="D128" s="28">
         <v>20135342</v>
       </c>
-      <c r="E128" s="2" t="s">
+      <c r="E128" s="28" t="s">
         <v>404</v>
       </c>
-      <c r="F128" s="2">
-        <v>3</v>
-      </c>
-      <c r="G128" s="2" t="s">
+      <c r="F128" s="28">
+        <v>3</v>
+      </c>
+      <c r="G128" s="28" t="s">
         <v>405</v>
       </c>
-      <c r="H128" s="1"/>
-      <c r="I128" s="3" t="s">
+      <c r="H128" s="29"/>
+      <c r="I128" s="30" t="s">
         <v>406</v>
       </c>
-      <c r="J128" s="6">
+      <c r="J128" s="31">
         <v>22</v>
       </c>
-      <c r="K128" s="6">
-        <v>1</v>
-      </c>
-      <c r="L128" s="6">
+      <c r="K128" s="31">
+        <v>1</v>
+      </c>
+      <c r="L128" s="31">
         <v>9</v>
       </c>
-      <c r="M128" s="6">
-        <v>5</v>
-      </c>
-      <c r="N128" s="6">
-        <v>0</v>
-      </c>
-      <c r="O128" s="6">
+      <c r="M128" s="31">
+        <v>5</v>
+      </c>
+      <c r="N128" s="31">
+        <v>0</v>
+      </c>
+      <c r="O128" s="31">
         <v>10</v>
       </c>
-      <c r="P128" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q128" s="6">
-        <v>0</v>
-      </c>
-      <c r="R128" s="6">
+      <c r="P128" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q128" s="31">
+        <v>0</v>
+      </c>
+      <c r="R128" s="31">
         <v>30</v>
       </c>
-      <c r="S128" s="6">
-        <v>1</v>
-      </c>
-      <c r="T128" s="6">
-        <v>0</v>
-      </c>
-      <c r="U128" s="6">
-        <v>5</v>
-      </c>
-      <c r="V128" s="6">
-        <v>4</v>
-      </c>
-      <c r="W128" s="6">
-        <v>3</v>
-      </c>
-      <c r="X128" s="6">
-        <v>2</v>
-      </c>
-      <c r="Y128" s="6">
-        <v>3</v>
-      </c>
-      <c r="Z128" s="6">
-        <v>3</v>
-      </c>
-      <c r="AA128" s="6">
-        <v>1</v>
-      </c>
-      <c r="AB128" s="6">
+      <c r="S128" s="31">
+        <v>1</v>
+      </c>
+      <c r="T128" s="31">
+        <v>0</v>
+      </c>
+      <c r="U128" s="31">
+        <v>5</v>
+      </c>
+      <c r="V128" s="31">
+        <v>4</v>
+      </c>
+      <c r="W128" s="31">
+        <v>3</v>
+      </c>
+      <c r="X128" s="31">
+        <v>2</v>
+      </c>
+      <c r="Y128" s="31">
+        <v>3</v>
+      </c>
+      <c r="Z128" s="31">
+        <v>3</v>
+      </c>
+      <c r="AA128" s="31">
+        <v>1</v>
+      </c>
+      <c r="AB128" s="31">
         <v>10</v>
       </c>
-      <c r="AC128" s="6">
-        <v>2</v>
-      </c>
-      <c r="AD128" s="6">
-        <v>3</v>
-      </c>
-      <c r="AE128" s="6">
-        <v>2</v>
-      </c>
-      <c r="AF128" s="6">
-        <v>1</v>
-      </c>
-      <c r="AG128" s="6">
+      <c r="AC128" s="31">
+        <v>2</v>
+      </c>
+      <c r="AD128" s="31">
+        <v>3</v>
+      </c>
+      <c r="AE128" s="31">
+        <v>2</v>
+      </c>
+      <c r="AF128" s="31">
+        <v>1</v>
+      </c>
+      <c r="AG128" s="31">
         <v>10</v>
       </c>
-      <c r="AH128" s="6">
-        <v>2</v>
-      </c>
-      <c r="AI128" s="6">
+      <c r="AH128" s="31">
+        <v>2</v>
+      </c>
+      <c r="AI128" s="31">
         <v>10</v>
       </c>
-      <c r="AJ128" s="6">
+      <c r="AJ128" s="31">
         <v>6</v>
       </c>
-      <c r="AK128" s="6">
-        <v>1</v>
-      </c>
-      <c r="AL128" s="6">
-        <v>4</v>
-      </c>
-      <c r="AM128" s="6">
-        <v>5</v>
-      </c>
-      <c r="AN128" s="6">
-        <v>2</v>
-      </c>
-      <c r="AO128" s="6">
-        <v>3</v>
-      </c>
-      <c r="AP128" s="6">
+      <c r="AK128" s="31">
+        <v>1</v>
+      </c>
+      <c r="AL128" s="31">
+        <v>4</v>
+      </c>
+      <c r="AM128" s="31">
+        <v>5</v>
+      </c>
+      <c r="AN128" s="31">
+        <v>2</v>
+      </c>
+      <c r="AO128" s="31">
+        <v>3</v>
+      </c>
+      <c r="AP128" s="31">
         <v>6</v>
       </c>
-      <c r="AQ128" s="6">
-        <v>5</v>
-      </c>
-      <c r="AR128" s="6">
-        <v>2</v>
-      </c>
-      <c r="AS128" s="6">
-        <v>4</v>
-      </c>
-      <c r="AT128" s="6">
-        <v>2</v>
-      </c>
-      <c r="AU128" s="6" t="s">
+      <c r="AQ128" s="31">
+        <v>5</v>
+      </c>
+      <c r="AR128" s="31">
+        <v>2</v>
+      </c>
+      <c r="AS128" s="31">
+        <v>4</v>
+      </c>
+      <c r="AT128" s="31">
+        <v>2</v>
+      </c>
+      <c r="AU128" s="31" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="129" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>125</v>
       </c>
@@ -18843,146 +18861,146 @@
         <v>582</v>
       </c>
     </row>
-    <row r="130" spans="1:47" ht="27.75" x14ac:dyDescent="0.3">
-      <c r="A130" s="2">
+    <row r="130" spans="1:47" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="28">
         <v>126</v>
       </c>
-      <c r="B130" s="1"/>
-      <c r="C130" s="2" t="s">
+      <c r="B130" s="29"/>
+      <c r="C130" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="D130" s="2">
+      <c r="D130" s="28">
         <v>20135343</v>
       </c>
-      <c r="E130" s="2" t="s">
+      <c r="E130" s="28" t="s">
         <v>410</v>
       </c>
-      <c r="F130" s="2">
-        <v>3</v>
-      </c>
-      <c r="G130" s="2" t="s">
+      <c r="F130" s="28">
+        <v>3</v>
+      </c>
+      <c r="G130" s="28" t="s">
         <v>411</v>
       </c>
-      <c r="H130" s="1"/>
-      <c r="I130" s="3" t="s">
+      <c r="H130" s="29"/>
+      <c r="I130" s="30" t="s">
         <v>412</v>
       </c>
-      <c r="J130" s="6">
+      <c r="J130" s="31">
         <v>22</v>
       </c>
-      <c r="K130" s="6">
-        <v>1</v>
-      </c>
-      <c r="L130" s="6">
+      <c r="K130" s="31">
+        <v>1</v>
+      </c>
+      <c r="L130" s="31">
         <v>9</v>
       </c>
-      <c r="M130" s="6">
-        <v>2</v>
-      </c>
-      <c r="N130" s="6">
-        <v>0</v>
-      </c>
-      <c r="O130" s="6">
+      <c r="M130" s="31">
+        <v>2</v>
+      </c>
+      <c r="N130" s="31">
+        <v>0</v>
+      </c>
+      <c r="O130" s="31">
         <v>6</v>
       </c>
-      <c r="P130" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q130" s="6">
-        <v>0</v>
-      </c>
-      <c r="R130" s="6">
-        <v>0</v>
-      </c>
-      <c r="S130" s="6">
-        <v>0</v>
-      </c>
-      <c r="T130" s="6">
+      <c r="P130" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q130" s="31">
+        <v>0</v>
+      </c>
+      <c r="R130" s="31">
+        <v>0</v>
+      </c>
+      <c r="S130" s="31">
+        <v>0</v>
+      </c>
+      <c r="T130" s="31">
         <v>30</v>
       </c>
-      <c r="U130" s="6">
-        <v>1</v>
-      </c>
-      <c r="V130" s="6">
-        <v>4</v>
-      </c>
-      <c r="W130" s="6">
-        <v>3</v>
-      </c>
-      <c r="X130" s="6">
-        <v>4</v>
-      </c>
-      <c r="Y130" s="6">
-        <v>3</v>
-      </c>
-      <c r="Z130" s="6">
-        <v>2</v>
-      </c>
-      <c r="AA130" s="6">
-        <v>3</v>
-      </c>
-      <c r="AB130" s="6">
-        <v>2</v>
-      </c>
-      <c r="AC130" s="6">
-        <v>0</v>
-      </c>
-      <c r="AD130" s="6">
-        <v>4</v>
-      </c>
-      <c r="AE130" s="6">
-        <v>1</v>
-      </c>
-      <c r="AF130" s="6">
-        <v>3</v>
-      </c>
-      <c r="AG130" s="6">
-        <v>2</v>
-      </c>
-      <c r="AH130" s="6">
-        <v>1</v>
-      </c>
-      <c r="AI130" s="6">
-        <v>3</v>
-      </c>
-      <c r="AJ130" s="6">
-        <v>2</v>
-      </c>
-      <c r="AK130" s="6">
-        <v>1</v>
-      </c>
-      <c r="AL130" s="6">
-        <v>5</v>
-      </c>
-      <c r="AM130" s="6">
-        <v>2</v>
-      </c>
-      <c r="AN130" s="6">
-        <v>1</v>
-      </c>
-      <c r="AO130" s="6">
-        <v>2</v>
-      </c>
-      <c r="AP130" s="6">
-        <v>1</v>
-      </c>
-      <c r="AQ130" s="6">
-        <v>2</v>
-      </c>
-      <c r="AR130" s="6">
-        <v>5</v>
-      </c>
-      <c r="AS130" s="6">
-        <v>5</v>
-      </c>
-      <c r="AT130" s="6">
-        <v>4</v>
-      </c>
-      <c r="AU130" s="6" t="s">
+      <c r="U130" s="31">
+        <v>1</v>
+      </c>
+      <c r="V130" s="31">
+        <v>4</v>
+      </c>
+      <c r="W130" s="31">
+        <v>3</v>
+      </c>
+      <c r="X130" s="31">
+        <v>4</v>
+      </c>
+      <c r="Y130" s="31">
+        <v>3</v>
+      </c>
+      <c r="Z130" s="31">
+        <v>2</v>
+      </c>
+      <c r="AA130" s="31">
+        <v>3</v>
+      </c>
+      <c r="AB130" s="31">
+        <v>2</v>
+      </c>
+      <c r="AC130" s="31">
+        <v>0</v>
+      </c>
+      <c r="AD130" s="31">
+        <v>4</v>
+      </c>
+      <c r="AE130" s="31">
+        <v>1</v>
+      </c>
+      <c r="AF130" s="31">
+        <v>3</v>
+      </c>
+      <c r="AG130" s="31">
+        <v>2</v>
+      </c>
+      <c r="AH130" s="31">
+        <v>1</v>
+      </c>
+      <c r="AI130" s="31">
+        <v>3</v>
+      </c>
+      <c r="AJ130" s="31">
+        <v>2</v>
+      </c>
+      <c r="AK130" s="31">
+        <v>1</v>
+      </c>
+      <c r="AL130" s="31">
+        <v>5</v>
+      </c>
+      <c r="AM130" s="31">
+        <v>2</v>
+      </c>
+      <c r="AN130" s="31">
+        <v>1</v>
+      </c>
+      <c r="AO130" s="31">
+        <v>2</v>
+      </c>
+      <c r="AP130" s="31">
+        <v>1</v>
+      </c>
+      <c r="AQ130" s="31">
+        <v>2</v>
+      </c>
+      <c r="AR130" s="31">
+        <v>5</v>
+      </c>
+      <c r="AS130" s="31">
+        <v>5</v>
+      </c>
+      <c r="AT130" s="31">
+        <v>4</v>
+      </c>
+      <c r="AU130" s="31" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="131" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>127</v>
       </c>
@@ -19111,7 +19129,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="132" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>128</v>
       </c>
@@ -19250,7 +19268,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="133" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>129</v>
       </c>
@@ -19379,7 +19397,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="134" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>130</v>
       </c>
@@ -19518,7 +19536,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="135" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>131</v>
       </c>
@@ -19653,7 +19671,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="136" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
         <v>132</v>
       </c>
@@ -19792,146 +19810,146 @@
         <v>582</v>
       </c>
     </row>
-    <row r="137" spans="1:47" ht="27.75" x14ac:dyDescent="0.3">
-      <c r="A137" s="2">
+    <row r="137" spans="1:47" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="28">
         <v>133</v>
       </c>
-      <c r="B137" s="1"/>
-      <c r="C137" s="2" t="s">
+      <c r="B137" s="29"/>
+      <c r="C137" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="D137" s="2">
+      <c r="D137" s="28">
         <v>20135347</v>
       </c>
-      <c r="E137" s="2" t="s">
+      <c r="E137" s="28" t="s">
         <v>431</v>
       </c>
-      <c r="F137" s="2">
-        <v>3</v>
-      </c>
-      <c r="G137" s="2" t="s">
+      <c r="F137" s="28">
+        <v>3</v>
+      </c>
+      <c r="G137" s="28" t="s">
         <v>432</v>
       </c>
-      <c r="H137" s="1"/>
-      <c r="I137" s="3" t="s">
+      <c r="H137" s="29"/>
+      <c r="I137" s="30" t="s">
         <v>433</v>
       </c>
-      <c r="J137" s="6">
+      <c r="J137" s="31">
         <v>23</v>
       </c>
-      <c r="K137" s="6">
-        <v>2</v>
-      </c>
-      <c r="L137" s="6">
+      <c r="K137" s="31">
+        <v>2</v>
+      </c>
+      <c r="L137" s="31">
         <v>9</v>
       </c>
-      <c r="M137" s="6">
-        <v>4</v>
-      </c>
-      <c r="N137" s="6">
-        <v>0</v>
-      </c>
-      <c r="O137" s="6">
+      <c r="M137" s="31">
+        <v>4</v>
+      </c>
+      <c r="N137" s="31">
+        <v>0</v>
+      </c>
+      <c r="O137" s="31">
         <v>8</v>
       </c>
-      <c r="P137" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q137" s="6">
-        <v>1</v>
-      </c>
-      <c r="R137" s="6">
-        <v>0</v>
-      </c>
-      <c r="S137" s="6">
-        <v>1</v>
-      </c>
-      <c r="T137" s="6">
-        <v>0</v>
-      </c>
-      <c r="U137" s="6">
-        <v>2</v>
-      </c>
-      <c r="V137" s="6">
-        <v>4</v>
-      </c>
-      <c r="W137" s="6">
-        <v>4</v>
-      </c>
-      <c r="X137" s="6">
+      <c r="P137" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q137" s="31">
+        <v>1</v>
+      </c>
+      <c r="R137" s="31">
+        <v>0</v>
+      </c>
+      <c r="S137" s="31">
+        <v>1</v>
+      </c>
+      <c r="T137" s="31">
+        <v>0</v>
+      </c>
+      <c r="U137" s="31">
+        <v>2</v>
+      </c>
+      <c r="V137" s="31">
+        <v>4</v>
+      </c>
+      <c r="W137" s="31">
+        <v>4</v>
+      </c>
+      <c r="X137" s="31">
         <v>6</v>
       </c>
-      <c r="Y137" s="6">
-        <v>1</v>
-      </c>
-      <c r="Z137" s="6">
-        <v>1</v>
-      </c>
-      <c r="AA137" s="6">
-        <v>3</v>
-      </c>
-      <c r="AB137" s="6">
+      <c r="Y137" s="31">
+        <v>1</v>
+      </c>
+      <c r="Z137" s="31">
+        <v>1</v>
+      </c>
+      <c r="AA137" s="31">
+        <v>3</v>
+      </c>
+      <c r="AB137" s="31">
         <v>15</v>
       </c>
-      <c r="AC137" s="6">
-        <v>0</v>
-      </c>
-      <c r="AD137" s="6">
-        <v>5</v>
-      </c>
-      <c r="AE137" s="6">
+      <c r="AC137" s="31">
+        <v>0</v>
+      </c>
+      <c r="AD137" s="31">
+        <v>5</v>
+      </c>
+      <c r="AE137" s="31">
         <v>11</v>
       </c>
-      <c r="AF137" s="6">
+      <c r="AF137" s="31">
         <v>13</v>
       </c>
-      <c r="AG137" s="6">
-        <v>1</v>
-      </c>
-      <c r="AH137" s="6">
+      <c r="AG137" s="31">
+        <v>1</v>
+      </c>
+      <c r="AH137" s="31">
         <v>10</v>
       </c>
-      <c r="AI137" s="6">
+      <c r="AI137" s="31">
         <v>8</v>
       </c>
-      <c r="AJ137" s="6">
-        <v>2</v>
-      </c>
-      <c r="AK137" s="6">
+      <c r="AJ137" s="31">
+        <v>2</v>
+      </c>
+      <c r="AK137" s="31">
         <v>6</v>
       </c>
-      <c r="AL137" s="6">
+      <c r="AL137" s="31">
         <v>10</v>
       </c>
-      <c r="AM137" s="6">
-        <v>2</v>
-      </c>
-      <c r="AN137" s="6">
-        <v>1</v>
-      </c>
-      <c r="AO137" s="6">
+      <c r="AM137" s="31">
+        <v>2</v>
+      </c>
+      <c r="AN137" s="31">
+        <v>1</v>
+      </c>
+      <c r="AO137" s="31">
         <v>6</v>
       </c>
-      <c r="AP137" s="6">
-        <v>1</v>
-      </c>
-      <c r="AQ137" s="6">
-        <v>1</v>
-      </c>
-      <c r="AR137" s="6">
-        <v>2</v>
-      </c>
-      <c r="AS137" s="6">
-        <v>4</v>
-      </c>
-      <c r="AT137" s="6">
-        <v>2</v>
-      </c>
-      <c r="AU137" s="6" t="s">
+      <c r="AP137" s="31">
+        <v>1</v>
+      </c>
+      <c r="AQ137" s="31">
+        <v>1</v>
+      </c>
+      <c r="AR137" s="31">
+        <v>2</v>
+      </c>
+      <c r="AS137" s="31">
+        <v>4</v>
+      </c>
+      <c r="AT137" s="31">
+        <v>2</v>
+      </c>
+      <c r="AU137" s="31" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="138" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>134</v>
       </c>
@@ -20066,7 +20084,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="139" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>135</v>
       </c>
@@ -20205,7 +20223,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="140" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <v>136</v>
       </c>
@@ -20338,7 +20356,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="141" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <v>137</v>
       </c>
@@ -20469,7 +20487,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="142" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
         <v>138</v>
       </c>
@@ -20598,7 +20616,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="143" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <v>139</v>
       </c>
@@ -20737,7 +20755,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="144" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <v>140</v>
       </c>
@@ -20872,7 +20890,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="145" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>141</v>
       </c>
@@ -20995,7 +21013,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="146" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <v>142</v>
       </c>
@@ -21134,7 +21152,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="147" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>143</v>
       </c>
@@ -21261,146 +21279,146 @@
         <v>581</v>
       </c>
     </row>
-    <row r="148" spans="1:47" ht="27.75" x14ac:dyDescent="0.3">
-      <c r="A148" s="2">
+    <row r="148" spans="1:47" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="28">
         <v>144</v>
       </c>
-      <c r="B148" s="1"/>
-      <c r="C148" s="2" t="s">
+      <c r="B148" s="29"/>
+      <c r="C148" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="D148" s="2">
+      <c r="D148" s="28">
         <v>20135350</v>
       </c>
-      <c r="E148" s="2" t="s">
+      <c r="E148" s="28" t="s">
         <v>464</v>
       </c>
-      <c r="F148" s="2">
-        <v>3</v>
-      </c>
-      <c r="G148" s="2" t="s">
+      <c r="F148" s="28">
+        <v>3</v>
+      </c>
+      <c r="G148" s="28" t="s">
         <v>465</v>
       </c>
-      <c r="H148" s="1"/>
-      <c r="I148" s="3" t="s">
+      <c r="H148" s="29"/>
+      <c r="I148" s="30" t="s">
         <v>466</v>
       </c>
-      <c r="J148" s="6">
+      <c r="J148" s="31">
         <v>23</v>
       </c>
-      <c r="K148" s="6">
-        <v>1</v>
-      </c>
-      <c r="L148" s="6">
+      <c r="K148" s="31">
+        <v>1</v>
+      </c>
+      <c r="L148" s="31">
         <v>9</v>
       </c>
-      <c r="M148" s="6">
-        <v>5</v>
-      </c>
-      <c r="N148" s="6">
-        <v>0</v>
-      </c>
-      <c r="O148" s="6">
+      <c r="M148" s="31">
+        <v>5</v>
+      </c>
+      <c r="N148" s="31">
+        <v>0</v>
+      </c>
+      <c r="O148" s="31">
         <v>10</v>
       </c>
-      <c r="P148" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q148" s="6">
-        <v>0</v>
-      </c>
-      <c r="R148" s="6">
+      <c r="P148" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q148" s="31">
+        <v>0</v>
+      </c>
+      <c r="R148" s="31">
         <v>30</v>
       </c>
-      <c r="S148" s="6">
-        <v>0</v>
-      </c>
-      <c r="T148" s="6">
+      <c r="S148" s="31">
+        <v>0</v>
+      </c>
+      <c r="T148" s="31">
         <v>30</v>
       </c>
-      <c r="U148" s="6">
-        <v>1</v>
-      </c>
-      <c r="V148" s="6">
-        <v>5</v>
-      </c>
-      <c r="W148" s="6">
-        <v>4</v>
-      </c>
-      <c r="X148" s="6">
+      <c r="U148" s="31">
+        <v>1</v>
+      </c>
+      <c r="V148" s="31">
+        <v>5</v>
+      </c>
+      <c r="W148" s="31">
+        <v>4</v>
+      </c>
+      <c r="X148" s="31">
         <v>7</v>
       </c>
-      <c r="Y148" s="6">
-        <v>2</v>
-      </c>
-      <c r="Z148" s="6">
-        <v>2</v>
-      </c>
-      <c r="AA148" s="6">
-        <v>3</v>
-      </c>
-      <c r="AB148" s="6">
-        <v>3</v>
-      </c>
-      <c r="AC148" s="6">
-        <v>0</v>
-      </c>
-      <c r="AD148" s="6">
-        <v>4</v>
-      </c>
-      <c r="AE148" s="6">
-        <v>1</v>
-      </c>
-      <c r="AF148" s="6">
-        <v>2</v>
-      </c>
-      <c r="AG148" s="6">
+      <c r="Y148" s="31">
+        <v>2</v>
+      </c>
+      <c r="Z148" s="31">
+        <v>2</v>
+      </c>
+      <c r="AA148" s="31">
+        <v>3</v>
+      </c>
+      <c r="AB148" s="31">
+        <v>3</v>
+      </c>
+      <c r="AC148" s="31">
+        <v>0</v>
+      </c>
+      <c r="AD148" s="31">
+        <v>4</v>
+      </c>
+      <c r="AE148" s="31">
+        <v>1</v>
+      </c>
+      <c r="AF148" s="31">
+        <v>2</v>
+      </c>
+      <c r="AG148" s="31">
         <v>13</v>
       </c>
-      <c r="AH148" s="6">
-        <v>1</v>
-      </c>
-      <c r="AI148" s="6">
-        <v>2</v>
-      </c>
-      <c r="AJ148" s="6">
+      <c r="AH148" s="31">
+        <v>1</v>
+      </c>
+      <c r="AI148" s="31">
+        <v>2</v>
+      </c>
+      <c r="AJ148" s="31">
         <v>13</v>
       </c>
-      <c r="AK148" s="6">
+      <c r="AK148" s="31">
         <v>8</v>
       </c>
-      <c r="AL148" s="6">
-        <v>5</v>
-      </c>
-      <c r="AM148" s="6">
-        <v>1</v>
-      </c>
-      <c r="AN148" s="6">
-        <v>2</v>
-      </c>
-      <c r="AO148" s="6">
-        <v>1</v>
-      </c>
-      <c r="AP148" s="6">
-        <v>2</v>
-      </c>
-      <c r="AQ148" s="6">
-        <v>1</v>
-      </c>
-      <c r="AR148" s="6">
-        <v>3</v>
-      </c>
-      <c r="AS148" s="6">
-        <v>4</v>
-      </c>
-      <c r="AT148" s="6">
-        <v>2</v>
-      </c>
-      <c r="AU148" s="6" t="s">
+      <c r="AL148" s="31">
+        <v>5</v>
+      </c>
+      <c r="AM148" s="31">
+        <v>1</v>
+      </c>
+      <c r="AN148" s="31">
+        <v>2</v>
+      </c>
+      <c r="AO148" s="31">
+        <v>1</v>
+      </c>
+      <c r="AP148" s="31">
+        <v>2</v>
+      </c>
+      <c r="AQ148" s="31">
+        <v>1</v>
+      </c>
+      <c r="AR148" s="31">
+        <v>3</v>
+      </c>
+      <c r="AS148" s="31">
+        <v>4</v>
+      </c>
+      <c r="AT148" s="31">
+        <v>2</v>
+      </c>
+      <c r="AU148" s="31" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="149" spans="1:47" ht="27.75" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>145</v>
       </c>
@@ -21529,7 +21547,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="150" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>146</v>
       </c>
@@ -21664,7 +21682,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="151" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <v>147</v>
       </c>
@@ -21793,7 +21811,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="152" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <v>148</v>
       </c>
@@ -21924,7 +21942,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="153" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <v>149</v>
       </c>
@@ -22045,7 +22063,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="154" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <v>150</v>
       </c>
@@ -22184,7 +22202,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="155" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>151</v>
       </c>
@@ -22249,7 +22267,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="156" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <v>152</v>
       </c>
@@ -22388,7 +22406,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="157" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
         <v>153</v>
       </c>
@@ -22519,7 +22537,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="158" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
         <v>154</v>
       </c>
@@ -22658,7 +22676,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="159" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>155</v>
       </c>
@@ -22797,7 +22815,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="160" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>156</v>
       </c>
@@ -22936,7 +22954,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="161" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <v>157</v>
       </c>
@@ -23069,7 +23087,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="162" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
         <v>158</v>
       </c>
@@ -23208,7 +23226,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="163" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <v>159</v>
       </c>
@@ -23347,7 +23365,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="164" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
         <v>160</v>
       </c>
@@ -23482,17 +23500,17 @@
         <v>582</v>
       </c>
     </row>
-    <row r="165" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A165" s="26">
+    <row r="165" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A165" s="11">
         <v>161</v>
       </c>
-      <c r="C165" s="26" t="s">
+      <c r="C165" s="11" t="s">
         <v>588</v>
       </c>
-      <c r="D165" s="26">
+      <c r="D165" s="11">
         <v>20131725</v>
       </c>
-      <c r="E165" s="26" t="s">
+      <c r="E165" s="11" t="s">
         <v>589</v>
       </c>
       <c r="J165" s="6">
@@ -23610,16 +23628,16 @@
         <v>587</v>
       </c>
     </row>
-    <row r="166" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:47" x14ac:dyDescent="0.25">
       <c r="AU166" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="AE3:AG3"/>
+    <mergeCell ref="AH3:AJ3"/>
     <mergeCell ref="AO3:AP3"/>
     <mergeCell ref="AQ3:AR3"/>
     <mergeCell ref="S3:T3"/>
@@ -23627,11 +23645,11 @@
     <mergeCell ref="AB2:AC2"/>
     <mergeCell ref="AE2:AJ2"/>
     <mergeCell ref="AO2:AR2"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="AE3:AG3"/>
-    <mergeCell ref="AH3:AJ3"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>